<commit_message>
completed version 1 of outage visuals
</commit_message>
<xml_diff>
--- a/Daily Data/OUTPUT/COAL/outages_20250314.xlsx
+++ b/Daily Data/OUTPUT/COAL/outages_20250314.xlsx
@@ -714,22 +714,22 @@
         <v>560</v>
       </c>
       <c r="C5" s="16" t="n">
-        <v>560</v>
+        <v>840</v>
       </c>
       <c r="D5" s="16" t="n">
-        <v>1280</v>
+        <v>1560</v>
       </c>
       <c r="E5" s="16" t="n">
-        <v>1280</v>
+        <v>1560</v>
       </c>
       <c r="F5" s="16" t="n">
-        <v>1280</v>
+        <v>1560</v>
       </c>
       <c r="G5" s="16" t="n">
-        <v>1280</v>
+        <v>1560</v>
       </c>
       <c r="H5" s="17" t="n">
-        <v>1630</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="6">
@@ -829,10 +829,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="26" t="n">
-        <v>45732</v>
+        <v>45738</v>
       </c>
       <c r="I11" s="32" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">

</xml_diff>